<commit_message>
update scripts for loading plan info
</commit_message>
<xml_diff>
--- a/Data_inputs/MISERS_PlanInfo.xlsx
+++ b/Data_inputs/MISERS_PlanInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="7" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -1140,8 +1140,8 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1670,9 +1670,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1694,10 +1691,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1706,8 +1703,11 @@
     <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3116,7 +3116,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,519 +3146,519 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="108"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
+      <c r="A5" s="107"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D6" s="109" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="108"/>
+      <c r="E6" s="107"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="111">
+      <c r="A7" s="110">
         <v>45</v>
       </c>
-      <c r="B7" s="112">
+      <c r="B7" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C7" s="113">
+      <c r="C7" s="112">
         <v>0</v>
       </c>
-      <c r="D7" s="113">
+      <c r="D7" s="112">
         <v>0</v>
       </c>
-      <c r="E7" s="108"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="111">
+      <c r="A8" s="110">
         <v>46</v>
       </c>
-      <c r="B8" s="112">
+      <c r="B8" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C8" s="113">
+      <c r="C8" s="112">
         <v>0</v>
       </c>
-      <c r="D8" s="113">
+      <c r="D8" s="112">
         <v>0</v>
       </c>
-      <c r="E8" s="108"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="111">
+      <c r="A9" s="110">
         <v>47</v>
       </c>
-      <c r="B9" s="112">
+      <c r="B9" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C9" s="113">
+      <c r="C9" s="112">
         <v>0</v>
       </c>
-      <c r="D9" s="113">
+      <c r="D9" s="112">
         <v>0</v>
       </c>
-      <c r="E9" s="108"/>
+      <c r="E9" s="107"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="111">
+      <c r="A10" s="110">
         <v>48</v>
       </c>
-      <c r="B10" s="112">
+      <c r="B10" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C10" s="113">
+      <c r="C10" s="112">
         <v>0</v>
       </c>
-      <c r="D10" s="113">
+      <c r="D10" s="112">
         <v>0</v>
       </c>
-      <c r="E10" s="108"/>
+      <c r="E10" s="107"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="111">
+      <c r="A11" s="110">
         <v>49</v>
       </c>
-      <c r="B11" s="112">
+      <c r="B11" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C11" s="113">
+      <c r="C11" s="112">
         <v>0</v>
       </c>
-      <c r="D11" s="113">
+      <c r="D11" s="112">
         <v>0</v>
       </c>
-      <c r="E11" s="108"/>
+      <c r="E11" s="107"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="111">
+      <c r="A12" s="110">
         <v>50</v>
       </c>
-      <c r="B12" s="112">
+      <c r="B12" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C12" s="113">
+      <c r="C12" s="112">
         <v>0</v>
       </c>
-      <c r="D12" s="113">
+      <c r="D12" s="112">
         <v>0</v>
       </c>
-      <c r="E12" s="108"/>
+      <c r="E12" s="107"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="111">
+      <c r="A13" s="110">
         <v>51</v>
       </c>
-      <c r="B13" s="112">
+      <c r="B13" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C13" s="112">
+      <c r="C13" s="111">
         <v>0.27</v>
       </c>
-      <c r="D13" s="113">
+      <c r="D13" s="112">
         <v>0</v>
       </c>
-      <c r="E13" s="108"/>
+      <c r="E13" s="107"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="111">
+      <c r="A14" s="110">
         <v>52</v>
       </c>
-      <c r="B14" s="112">
+      <c r="B14" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C14" s="112">
+      <c r="C14" s="111">
         <v>0.21</v>
       </c>
-      <c r="D14" s="113">
+      <c r="D14" s="112">
         <v>0</v>
       </c>
-      <c r="E14" s="108"/>
+      <c r="E14" s="107"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="111">
+      <c r="A15" s="110">
         <v>53</v>
       </c>
-      <c r="B15" s="112">
+      <c r="B15" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C15" s="112">
+      <c r="C15" s="111">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D15" s="113">
+      <c r="D15" s="112">
         <v>0</v>
       </c>
-      <c r="E15" s="108"/>
+      <c r="E15" s="107"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="111">
+      <c r="A16" s="110">
         <v>54</v>
       </c>
-      <c r="B16" s="112">
+      <c r="B16" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C16" s="112">
+      <c r="C16" s="111">
         <v>0.16</v>
       </c>
-      <c r="D16" s="113">
+      <c r="D16" s="112">
         <v>0</v>
       </c>
-      <c r="E16" s="108"/>
+      <c r="E16" s="107"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="111">
+      <c r="A17" s="110">
         <v>55</v>
       </c>
-      <c r="B17" s="112">
+      <c r="B17" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C17" s="112">
+      <c r="C17" s="111">
         <v>0.16</v>
       </c>
-      <c r="D17" s="112">
+      <c r="D17" s="111">
         <v>0.15</v>
       </c>
-      <c r="E17" s="108"/>
+      <c r="E17" s="107"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="111">
+      <c r="A18" s="110">
         <v>56</v>
       </c>
-      <c r="B18" s="112">
+      <c r="B18" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C18" s="112">
+      <c r="C18" s="111">
         <v>0.22</v>
       </c>
-      <c r="D18" s="112">
+      <c r="D18" s="111">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E18" s="108"/>
+      <c r="E18" s="107"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="111">
+      <c r="A19" s="110">
         <v>57</v>
       </c>
-      <c r="B19" s="112">
+      <c r="B19" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C19" s="112">
+      <c r="C19" s="111">
         <v>0.15</v>
       </c>
-      <c r="D19" s="112">
+      <c r="D19" s="111">
         <v>0.1</v>
       </c>
-      <c r="E19" s="108"/>
+      <c r="E19" s="107"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="111">
+      <c r="A20" s="110">
         <v>58</v>
       </c>
-      <c r="B20" s="112">
+      <c r="B20" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C20" s="112">
+      <c r="C20" s="111">
         <v>0.12</v>
       </c>
-      <c r="D20" s="112">
+      <c r="D20" s="111">
         <v>0.1</v>
       </c>
-      <c r="E20" s="108"/>
+      <c r="E20" s="107"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="111">
+      <c r="A21" s="110">
         <v>59</v>
       </c>
-      <c r="B21" s="112">
+      <c r="B21" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C21" s="112">
+      <c r="C21" s="111">
         <v>0.12</v>
       </c>
-      <c r="D21" s="112">
+      <c r="D21" s="111">
         <v>0.11</v>
       </c>
-      <c r="E21" s="108"/>
+      <c r="E21" s="107"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="111">
+      <c r="A22" s="110">
         <v>60</v>
       </c>
-      <c r="B22" s="112">
+      <c r="B22" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C22" s="112">
+      <c r="C22" s="111">
         <v>0.18</v>
       </c>
-      <c r="D22" s="112">
+      <c r="D22" s="111">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E22" s="108"/>
+      <c r="E22" s="107"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="111">
+      <c r="A23" s="110">
         <v>61</v>
       </c>
-      <c r="B23" s="112">
+      <c r="B23" s="111">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C23" s="112">
+      <c r="C23" s="111">
         <v>0.18</v>
       </c>
-      <c r="D23" s="112">
+      <c r="D23" s="111">
         <v>0.13</v>
       </c>
-      <c r="E23" s="108"/>
+      <c r="E23" s="107"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="111">
+      <c r="A24" s="110">
         <v>62</v>
       </c>
-      <c r="B24" s="112">
+      <c r="B24" s="111">
         <v>0.5</v>
       </c>
-      <c r="C24" s="112">
+      <c r="C24" s="111">
         <v>0.32</v>
       </c>
-      <c r="D24" s="112">
+      <c r="D24" s="111">
         <v>0.22</v>
       </c>
-      <c r="E24" s="108"/>
+      <c r="E24" s="107"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="111">
+      <c r="A25" s="110">
         <v>63</v>
       </c>
-      <c r="B25" s="112">
+      <c r="B25" s="111">
         <v>0.4</v>
       </c>
-      <c r="C25" s="112">
+      <c r="C25" s="111">
         <v>0.24</v>
       </c>
-      <c r="D25" s="112">
+      <c r="D25" s="111">
         <v>0.19</v>
       </c>
-      <c r="E25" s="108"/>
+      <c r="E25" s="107"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="111">
+      <c r="A26" s="110">
         <v>64</v>
       </c>
-      <c r="B26" s="112">
+      <c r="B26" s="111">
         <v>0.4</v>
       </c>
-      <c r="C26" s="112">
+      <c r="C26" s="111">
         <v>0.22</v>
       </c>
-      <c r="D26" s="112">
+      <c r="D26" s="111">
         <v>0.16</v>
       </c>
-      <c r="E26" s="108"/>
+      <c r="E26" s="107"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="111">
+      <c r="A27" s="110">
         <v>65</v>
       </c>
-      <c r="B27" s="112">
+      <c r="B27" s="111">
         <v>0.6</v>
       </c>
-      <c r="C27" s="112">
+      <c r="C27" s="111">
         <v>0.16</v>
       </c>
-      <c r="D27" s="112">
+      <c r="D27" s="111">
         <v>0.25</v>
       </c>
-      <c r="E27" s="108"/>
+      <c r="E27" s="107"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="111">
+      <c r="A28" s="110">
         <v>66</v>
       </c>
-      <c r="B28" s="112">
+      <c r="B28" s="111">
         <v>0.5</v>
       </c>
-      <c r="C28" s="112">
+      <c r="C28" s="111">
         <v>0.22</v>
       </c>
-      <c r="D28" s="112">
+      <c r="D28" s="111">
         <v>0.22</v>
       </c>
-      <c r="E28" s="108"/>
+      <c r="E28" s="107"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="111">
+      <c r="A29" s="110">
         <v>67</v>
       </c>
-      <c r="B29" s="112">
+      <c r="B29" s="111">
         <v>0.5</v>
       </c>
-      <c r="C29" s="112">
+      <c r="C29" s="111">
         <v>0.3</v>
       </c>
-      <c r="D29" s="112">
+      <c r="D29" s="111">
         <v>0.21</v>
       </c>
-      <c r="E29" s="108"/>
+      <c r="E29" s="107"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="111">
+      <c r="A30" s="110">
         <v>68</v>
       </c>
-      <c r="B30" s="112">
+      <c r="B30" s="111">
         <v>0.5</v>
       </c>
-      <c r="C30" s="112">
+      <c r="C30" s="111">
         <v>0.4</v>
       </c>
-      <c r="D30" s="112">
+      <c r="D30" s="111">
         <v>0.2</v>
       </c>
-      <c r="E30" s="108"/>
+      <c r="E30" s="107"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="111">
+      <c r="A31" s="110">
         <v>69</v>
       </c>
-      <c r="B31" s="112">
+      <c r="B31" s="111">
         <v>0.5</v>
       </c>
-      <c r="C31" s="112">
+      <c r="C31" s="111">
         <v>0.5</v>
       </c>
-      <c r="D31" s="112">
+      <c r="D31" s="111">
         <v>0.22</v>
       </c>
-      <c r="E31" s="108"/>
+      <c r="E31" s="107"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="111">
+      <c r="A32" s="110">
         <v>70</v>
       </c>
-      <c r="B32" s="112">
+      <c r="B32" s="111">
         <v>1</v>
       </c>
-      <c r="C32" s="112">
+      <c r="C32" s="111">
         <v>1</v>
       </c>
-      <c r="D32" s="112">
+      <c r="D32" s="111">
         <v>0.5</v>
       </c>
-      <c r="E32" s="108"/>
+      <c r="E32" s="107"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="111">
+      <c r="A33" s="110">
         <v>71</v>
       </c>
-      <c r="B33" s="112">
+      <c r="B33" s="111">
         <v>1</v>
       </c>
-      <c r="C33" s="112">
+      <c r="C33" s="111">
         <v>1</v>
       </c>
-      <c r="D33" s="112">
+      <c r="D33" s="111">
         <v>0.6</v>
       </c>
-      <c r="E33" s="108"/>
+      <c r="E33" s="107"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="111">
+      <c r="A34" s="110">
         <v>72</v>
       </c>
-      <c r="B34" s="112">
+      <c r="B34" s="111">
         <v>1</v>
       </c>
-      <c r="C34" s="112">
+      <c r="C34" s="111">
         <v>1</v>
       </c>
-      <c r="D34" s="112">
+      <c r="D34" s="111">
         <v>0.7</v>
       </c>
-      <c r="E34" s="108"/>
+      <c r="E34" s="107"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="111">
+      <c r="A35" s="110">
         <v>73</v>
       </c>
-      <c r="B35" s="112">
+      <c r="B35" s="111">
         <v>1</v>
       </c>
-      <c r="C35" s="112">
+      <c r="C35" s="111">
         <v>1</v>
       </c>
-      <c r="D35" s="112">
+      <c r="D35" s="111">
         <v>0.8</v>
       </c>
-      <c r="E35" s="108"/>
+      <c r="E35" s="107"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="111">
+      <c r="A36" s="110">
         <v>74</v>
       </c>
-      <c r="B36" s="112">
+      <c r="B36" s="111">
         <v>1</v>
       </c>
-      <c r="C36" s="112">
+      <c r="C36" s="111">
         <v>1</v>
       </c>
-      <c r="D36" s="112">
+      <c r="D36" s="111">
         <v>0.9</v>
       </c>
-      <c r="E36" s="108"/>
+      <c r="E36" s="107"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="111">
+      <c r="A37" s="110">
         <v>75</v>
       </c>
-      <c r="B37" s="112">
+      <c r="B37" s="111">
         <v>1</v>
       </c>
-      <c r="C37" s="112">
+      <c r="C37" s="111">
         <v>1</v>
       </c>
-      <c r="D37" s="112">
+      <c r="D37" s="111">
         <v>1</v>
       </c>
-      <c r="E37" s="108"/>
+      <c r="E37" s="107"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="109"/>
-      <c r="B38" s="109"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="109"/>
-      <c r="E38" s="108"/>
+      <c r="A38" s="108"/>
+      <c r="B38" s="108"/>
+      <c r="C38" s="108"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="107"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="108"/>
-      <c r="B39" s="108"/>
-      <c r="C39" s="108"/>
-      <c r="D39" s="108"/>
-      <c r="E39" s="108"/>
+      <c r="A39" s="107"/>
+      <c r="B39" s="107"/>
+      <c r="C39" s="107"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="107"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="108"/>
-      <c r="B40" s="108"/>
-      <c r="C40" s="108"/>
-      <c r="D40" s="108"/>
-      <c r="E40" s="108"/>
+      <c r="A40" s="107"/>
+      <c r="B40" s="107"/>
+      <c r="C40" s="107"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="107"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="108"/>
-      <c r="B41" s="108"/>
-      <c r="C41" s="108"/>
-      <c r="D41" s="108"/>
-      <c r="E41" s="108"/>
+      <c r="A41" s="107"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="107"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="107"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3789,8 +3789,8 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
-      <c r="B7" s="107"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="121"/>
     </row>
     <row r="8" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -3877,7 +3877,7 @@
       <c r="A6" s="40">
         <v>0</v>
       </c>
-      <c r="B6" s="114">
+      <c r="B6" s="113">
         <v>0.12</v>
       </c>
       <c r="E6" s="38"/>
@@ -3889,7 +3889,7 @@
       <c r="A7" s="40">
         <v>1</v>
       </c>
-      <c r="B7" s="114">
+      <c r="B7" s="113">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="E7" s="39"/>
@@ -3901,7 +3901,7 @@
       <c r="A8" s="40">
         <v>2</v>
       </c>
-      <c r="B8" s="114">
+      <c r="B8" s="113">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="C8" s="18"/>
@@ -3914,7 +3914,7 @@
       <c r="A9" s="40">
         <v>3</v>
       </c>
-      <c r="B9" s="114">
+      <c r="B9" s="113">
         <v>0.05</v>
       </c>
       <c r="C9" s="18"/>
@@ -3927,7 +3927,7 @@
       <c r="A10" s="40">
         <v>4</v>
       </c>
-      <c r="B10" s="114">
+      <c r="B10" s="113">
         <v>0.04</v>
       </c>
       <c r="C10" s="18"/>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
-      <c r="B11" s="115"/>
+      <c r="B11" s="114"/>
       <c r="C11" s="18"/>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
@@ -4071,38 +4071,38 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="115" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="116">
+      <c r="A6" s="115">
         <v>20</v>
       </c>
-      <c r="B6" s="117">
+      <c r="B6" s="116">
         <v>0.04</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="116">
+      <c r="A7" s="115">
         <v>25</v>
       </c>
-      <c r="B7" s="118">
+      <c r="B7" s="117">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="116">
+      <c r="A8" s="115">
         <v>30</v>
       </c>
-      <c r="B8" s="118">
+      <c r="B8" s="117">
         <v>2.8199999999999999E-2</v>
       </c>
       <c r="C8" s="18"/>
@@ -4110,10 +4110,10 @@
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="116">
+      <c r="A9" s="115">
         <v>35</v>
       </c>
-      <c r="B9" s="118">
+      <c r="B9" s="117">
         <v>2.3800000000000002E-2</v>
       </c>
       <c r="C9" s="18"/>
@@ -4121,10 +4121,10 @@
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="116">
+      <c r="A10" s="115">
         <v>40</v>
       </c>
-      <c r="B10" s="118">
+      <c r="B10" s="117">
         <v>2.06E-2</v>
       </c>
       <c r="C10" s="18"/>
@@ -4132,10 +4132,10 @@
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="116">
+      <c r="A11" s="115">
         <v>45</v>
       </c>
-      <c r="B11" s="118">
+      <c r="B11" s="117">
         <v>1.84E-2</v>
       </c>
       <c r="C11" s="18"/>
@@ -4143,10 +4143,10 @@
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="116">
+      <c r="A12" s="115">
         <v>50</v>
       </c>
-      <c r="B12" s="118">
+      <c r="B12" s="117">
         <v>1.6799999999999999E-2</v>
       </c>
       <c r="C12" s="18"/>
@@ -4154,10 +4154,10 @@
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="116">
+      <c r="A13" s="115">
         <v>55</v>
       </c>
-      <c r="B13" s="118">
+      <c r="B13" s="117">
         <v>1.6E-2</v>
       </c>
       <c r="C13" s="18"/>
@@ -4165,10 +4165,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="116">
+      <c r="A14" s="115">
         <v>60</v>
       </c>
-      <c r="B14" s="118">
+      <c r="B14" s="117">
         <v>1.6E-2</v>
       </c>
       <c r="C14" s="18"/>
@@ -4314,7 +4314,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4352,129 +4352,129 @@
       <c r="D3" s="17"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="119" t="s">
+      <c r="A5" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="118" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="118" t="s">
         <v>167</v>
       </c>
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="120">
+      <c r="A6" s="119">
         <v>25</v>
       </c>
-      <c r="B6" s="121">
+      <c r="B6" s="120">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="C6" s="121">
+      <c r="C6" s="120">
         <v>0</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="120">
+      <c r="A7" s="119">
         <v>30</v>
       </c>
-      <c r="B7" s="121">
+      <c r="B7" s="120">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C7" s="121">
+      <c r="C7" s="120">
         <v>1E-4</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="120">
+      <c r="A8" s="119">
         <v>35</v>
       </c>
-      <c r="B8" s="121">
+      <c r="B8" s="120">
         <v>1E-3</v>
       </c>
-      <c r="C8" s="121">
+      <c r="C8" s="120">
         <v>1E-4</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="120">
+      <c r="A9" s="119">
         <v>40</v>
       </c>
-      <c r="B9" s="121">
+      <c r="B9" s="120">
         <v>2E-3</v>
       </c>
-      <c r="C9" s="121">
+      <c r="C9" s="120">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="120">
+      <c r="A10" s="119">
         <v>45</v>
       </c>
-      <c r="B10" s="121">
+      <c r="B10" s="120">
         <v>3.4000000000000002E-3</v>
       </c>
-      <c r="C10" s="121">
+      <c r="C10" s="120">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="120">
+      <c r="A11" s="119">
         <v>50</v>
       </c>
-      <c r="B11" s="121">
+      <c r="B11" s="120">
         <v>4.6999999999999993E-3</v>
       </c>
-      <c r="C11" s="121">
+      <c r="C11" s="120">
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="120">
+      <c r="A12" s="119">
         <v>55</v>
       </c>
-      <c r="B12" s="121">
+      <c r="B12" s="120">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="C12" s="121">
+      <c r="C12" s="120">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="120">
+      <c r="A13" s="119">
         <v>60</v>
       </c>
-      <c r="B13" s="121">
+      <c r="B13" s="120">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="C13" s="121">
+      <c r="C13" s="120">
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="120">
+      <c r="A14" s="119">
         <v>65</v>
       </c>
-      <c r="B14" s="121">
+      <c r="B14" s="120">
         <v>2.3E-2</v>
       </c>
-      <c r="C14" s="121">
+      <c r="C14" s="120">
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="D14" s="20"/>
@@ -4590,8 +4590,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4698,8 +4698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5003,7 +5003,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>